<commit_message>
Laporan, Rabu 19 Februari 2025
</commit_message>
<xml_diff>
--- a/Laporan Pemodelan Matematika.xlsx
+++ b/Laporan Pemodelan Matematika.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mahasiswa\Pictures\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f605dad1326c742d/Kuliah/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{49D19714-131D-44E7-9769-6A6B6EDD0C34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3C1D44E6-6148-4994-A51A-4D0319E87832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{68D7E6CB-B78C-46F1-AB10-67F2F333EF9B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{68D7E6CB-B78C-46F1-AB10-67F2F333EF9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -47,10 +47,10 @@
   </si>
   <si>
     <t>Mencari 5 artikel yang berkaitan dengan pemodelan matematika dengan tema tentang laju pertumbuhan diantaranya : 
-1. Pemodelan Matematika Terhadap Kecanduan Game Online (https://ejurnal.methodist.ac.id/index.php/methoda/article/view/2773/1857), 
+1. Proyeksi Pertumbuhan Penduduk Sulawesi Tenggara dengan menggunakan model eksponensial dan model logistik (https://jaf.uho.ac.id/index.php/JAFUHO/article/view/15/6), 
 2. Pengaruh Jumlah Penduduk Miskin (https://journals.unisba.ac.id/index.php/JRIEB/article/view/401), 
 3. Pengaruh Upah Minimum (https://journals.unisba.ac.id/index.php/JRIEB/article/view/1911), 
-4. Model Matematika Predator dan Prey Terinfeksi dengan Kontrol Pestisida pada Penyebaran Hama Wereng Batang Cokelat di Kabupaten Bantul (https://www.fourier.or.id/index.php/FOURIER/article/view/93/90), 
+4. Proyeksi Pertumbuhan Mobil Pribadi Roda Empat (Plat Hitam) Kota Manado Menggunakan Persamaan Differensial Model Pertumbuhan Populasi Kontinu (Model Logistik) (https://ejournal.unsrat.ac.id/v3/index.php/decartesian/article/view/14017/13590), 
 5. Model Pertumbuhan Populasi Malthus (https://media.neliti.com/media/publications/185154-ID-kestabilan-populasi-model-lotka-volterra.pdf).</t>
   </si>
 </sst>
@@ -430,7 +430,7 @@
   <dimension ref="B3:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -447,7 +447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="210" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" ht="180" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>

</xml_diff>